<commit_message>
Update Glosario Ranking Muni_2018_GT.xlsx
</commit_message>
<xml_diff>
--- a/Guatemala/Glosario Ranking Muni_2018_GT.xlsx
+++ b/Guatemala/Glosario Ranking Muni_2018_GT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA INTELLIGENCE Dropbox\Diseño DATA's\DATA-MUNI\Guatemala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F15A94-5F45-4E4D-AD7E-86D37D333AC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7B741A-E4D1-4CE7-958A-31705D79E9DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1D4769EB-C3C3-42EF-8AF0-E54E6B5F48E8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>IGA</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Índice de Información a la Ciudadanía</t>
   </si>
   <si>
-    <t>Índice de Servicios Públicos</t>
-  </si>
-  <si>
     <t>Índice de Gestión Financiera</t>
   </si>
   <si>
@@ -81,10 +78,110 @@
     <t xml:space="preserve">El índice general está compuesto por seis índices temáticos que contienen indicadores con igual ponderación, reflejando la misma importancia de cada uno de ellos. Es un resumen de los 31indicadores que ubica a las municipalidades que tienen o están más cerca de las mejores prácticas en todos los temas analizados, y sintetiza el trabajo municipal en materia de gestión para la gobernabilidad. </t>
   </si>
   <si>
-    <t>IGGM</t>
-  </si>
-  <si>
     <t xml:space="preserve">Índice General de Gestión Municipal </t>
+  </si>
+  <si>
+    <t>1. Número de reuniones del COMUDE en el año de la medición</t>
+  </si>
+  <si>
+    <t>Indicadores</t>
+  </si>
+  <si>
+    <t>2. Participación de Alcaldes, Concejales y Síndicos determinados o designados en el COMUDE</t>
+  </si>
+  <si>
+    <t>3. Participación de organizaciones de jóvenes, mujeres, pueblos mayas, xincas, garífunas, y otras organizaciones en el COMUDE</t>
+  </si>
+  <si>
+    <t>4. Representatividad territorial del COMUDE</t>
+  </si>
+  <si>
+    <t>5. Funcionamiento del COMUDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muestra la capacidad de los municipios para proporcionar información a la ciudadanía por medio del proceso de rendición de cuentas ante el COMUDE y de la información pública que está disponible. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Rendición de cuentas cuatrimestrales y anual al COMUDE, enfocadas a resultados </t>
+  </si>
+  <si>
+    <t>2. Información Presupuestaria y otra información brindada a la ciudadanía, y disponible en medios locales de información</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Relación de monto contratado a través de Guatecompras y el total del presupuesto de egresos. </t>
+  </si>
+  <si>
+    <t>3. Información pública de oficio actualizada, y disponible en todo momento, de acuerdo a la Ley de Acceso a la Información Pública (LAIP) y uso de internet</t>
+  </si>
+  <si>
+    <t>Índice de Gestión de Servicios Públicos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Existencia de elementos de atención municipal orientada al ciuadano </t>
+  </si>
+  <si>
+    <t>2. Gestión del recurso humano</t>
+  </si>
+  <si>
+    <t>3. Existencia de oficinas municipales con instrumentos de gestión</t>
+  </si>
+  <si>
+    <t>Mide la eficiencia en el uso de los recursos financieros que las municipalidades reciben del gobierno central, los que recaudan por sí mismos y otras fuentes de financiamiento en función de la forma y el destino en que se efectúa el gasto.</t>
+  </si>
+  <si>
+    <t>3. Indicador de la existencia de oficinas municipales con instrumentos de gestión</t>
+  </si>
+  <si>
+    <t>2. Indicador Gestión del recurso humano</t>
+  </si>
+  <si>
+    <t>1. Indicador de la existencia de elementos de atención municipal orientada al ciudadano</t>
+  </si>
+  <si>
+    <t>1. Indicador de autonomía financiera municipal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Indicador de ingresos propios por habitante (sin regalías) </t>
+  </si>
+  <si>
+    <t>3. Indicador Ingresos del Impuesto Único sobre Inmuebles (IUSI) respecto a ingresos propios (sin regalías)</t>
+  </si>
+  <si>
+    <t>4. Indicador de la inversión anual en capital fijo por habitante</t>
+  </si>
+  <si>
+    <t>5. Indicador de la inversión anual en capital fijo con ingresos propios</t>
+  </si>
+  <si>
+    <t>6. Indicador de la inversión anual en capital fijo con transferencia</t>
+  </si>
+  <si>
+    <t>7. Indicador de independencia financiera por endeudamiento público</t>
+  </si>
+  <si>
+    <t>Analiza la forma en que la planificación de las municipalidades incide en el desarrollo del municipio en relación con el presupuesto municipal, indagando cómo controla y gestiona el territorio de manera ordenada y cómo aplica en esa planificación la gestión del riesgo.</t>
+  </si>
+  <si>
+    <t>1. Ejecución del Plan Operativo Anual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Presupuesto de egresos relacionado a competencias municipales, vinculadas a prioridades nacionales </t>
+  </si>
+  <si>
+    <t>4. Institucionalización de la gestión ordenada del territorio</t>
+  </si>
+  <si>
+    <t>5. Acciones para la gestión ordenada del territorio</t>
+  </si>
+  <si>
+    <t>6. Análisis de la gestión de riesgo en la formulación de proyectos</t>
+  </si>
+  <si>
+    <t>7. Ingresos por Servicios Ambientales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Relación plan de desarrollo municipal y ordenamiento 
+territorial (PDM-OT), plan estratégico (PEI), plan operativo multianual (POM) y el plan operativo anual (POA). </t>
   </si>
 </sst>
 </file>
@@ -107,18 +204,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -144,7 +235,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -461,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8EF3876-72B3-4ED7-B0A4-294D8F4A2000}">
-  <dimension ref="B2:D8"/>
+  <dimension ref="B1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
@@ -473,23 +564,27 @@
     <col min="2" max="2" width="29.90625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.453125" style="3" customWidth="1"/>
     <col min="4" max="4" width="65.81640625" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="10.90625" style="1"/>
+    <col min="5" max="5" width="44.6328125" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="10.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="65" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" ht="65" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>15</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C2" s="4"/>
       <c r="D2" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" ht="39" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="39" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>0</v>
@@ -497,51 +592,197 @@
       <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" ht="78" x14ac:dyDescent="0.35">
-      <c r="B4" s="1" t="s">
+      <c r="E3" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E4" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="26" x14ac:dyDescent="0.35">
+      <c r="E5" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="78" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" ht="104" x14ac:dyDescent="0.35">
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="C6" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="E6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="26" x14ac:dyDescent="0.35">
+      <c r="D7" s="1"/>
+      <c r="E7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E8" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E9" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C10" s="1"/>
+      <c r="E10" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="39" x14ac:dyDescent="0.35">
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="39" x14ac:dyDescent="0.35">
+      <c r="E12" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="39" x14ac:dyDescent="0.35">
+      <c r="E13" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="26" x14ac:dyDescent="0.35">
+      <c r="E14" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="104" x14ac:dyDescent="0.35">
+      <c r="B15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E16" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="26" x14ac:dyDescent="0.35">
+      <c r="E17" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="39" x14ac:dyDescent="0.35">
+      <c r="B18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="1"/>
+      <c r="E19" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E20" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="26" x14ac:dyDescent="0.35">
+      <c r="E21" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="26" x14ac:dyDescent="0.35">
+      <c r="E22" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="26" x14ac:dyDescent="0.35">
+      <c r="C23" s="1"/>
+      <c r="E23" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="26" x14ac:dyDescent="0.35">
+      <c r="E24" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="52" x14ac:dyDescent="0.35">
+      <c r="B25" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>0</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E26" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="26" x14ac:dyDescent="0.35">
+      <c r="E27" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E28" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E29" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="26" x14ac:dyDescent="0.35">
+      <c r="E30" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="E31" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>